<commit_message>
docs: Update Cell Formula, added header.
</commit_message>
<xml_diff>
--- a/monthly_stock_contribution.xlsx
+++ b/monthly_stock_contribution.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t xml:space="preserve">Monthly Stock Contribution Compared With Ordinary Stock Purchase (Does not include handling Fees)</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gain / Loss (include dividend)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordinary Stock Purchase (Exclude Handling Fees)</t>
   </si>
   <si>
     <t xml:space="preserve">Buy Stock HSBC Holdings</t>
@@ -436,14 +439,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,6 +451,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,6 +473,10 @@
     </xf>
     <xf numFmtId="167" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -666,7 +669,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,153 +1016,158 @@
         <v>31</v>
       </c>
       <c r="D21" s="25" t="n">
-        <f aca="false">(D20*B19 - B5)</f>
-        <v>5247.01136446636</v>
+        <f aca="false">(B21- B5)</f>
+        <v>5247.0113644664</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F21" s="25" t="n">
-        <f aca="false">(D20*B19 - B5) + E20</f>
-        <v>8126.94492985165</v>
+        <f aca="false">(B21 - B5) + E20</f>
+        <v>8126.94492985169</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="28"/>
+      <c r="A23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="28" t="s">
         <v>34</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="C24" s="15" t="n">
         <v>800</v>
       </c>
-      <c r="D24" s="28"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="30"/>
-      <c r="B25" s="32" t="s">
-        <v>35</v>
+      <c r="A25" s="28"/>
+      <c r="B25" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="C25" s="9" t="n">
         <v>59.3</v>
       </c>
-      <c r="D25" s="28"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="27"/>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30"/>
-      <c r="B26" s="32" t="s">
+      <c r="A26" s="28"/>
+      <c r="B26" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="33" t="n">
+      <c r="C26" s="32" t="n">
         <f aca="false">C24*C25</f>
         <v>47440</v>
       </c>
-      <c r="D26" s="28"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="27"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>34</v>
+      <c r="A27" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>35</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>800</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="31"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="34"/>
-      <c r="B28" s="36" t="s">
-        <v>37</v>
+      <c r="A28" s="33"/>
+      <c r="B28" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="C28" s="9" t="n">
         <v>71.5</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="31"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="34"/>
-      <c r="B29" s="36" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="9" t="n">
         <f aca="false">C27*C28</f>
         <v>57200</v>
       </c>
-      <c r="D29" s="28"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="27"/>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="36" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="25" t="n">
         <f aca="false">C29-C26</f>
         <v>9760</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="31"/>
       <c r="E30" s="27"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="36" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="25" t="n">
         <f aca="false">(C29-C26)+((F5/10*3)*C24)+((F5/10*2.1)*C24)+((F5/10*1)*C24)+((F5/10*1)*C24)+((F5/10*1)*C24)</f>
         <v>14794.96</v>
       </c>
-      <c r="D31" s="28"/>
+      <c r="D31" s="31"/>
       <c r="E31" s="27"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="28"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="27"/>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="38"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="28"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="27"/>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="38"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="28"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A31"/>

</xml_diff>